<commit_message>
add new img and new db
</commit_message>
<xml_diff>
--- a/dummy/in4.xlsx
+++ b/dummy/in4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Lập trình web\assignment\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\GitHub\HCMG\dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBB2CFB-74DC-4F4B-91C7-FB2894D4A105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAED9ED-EF6D-4735-9666-53349E0A3AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3708" yWindow="1764" windowWidth="15372" windowHeight="8268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="1704" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Eden Ring</t>
   </si>
@@ -39,64 +39,55 @@
     <t>Halo Infinite</t>
   </si>
   <si>
-    <t>thể loại</t>
-  </si>
-  <si>
-    <t>Hành động</t>
-  </si>
-  <si>
-    <t>nhà sản xuất</t>
-  </si>
-  <si>
-    <t>343 Industries</t>
-  </si>
-  <si>
     <t>Ghostwire: Tokyo</t>
   </si>
   <si>
-    <t>Tango Gameworks</t>
-  </si>
-  <si>
     <t>ELEX II</t>
   </si>
   <si>
-    <t>Hành động Phiêu lưu Nhập vai - RPG</t>
-  </si>
-  <si>
-    <t>Piranha Bytes</t>
-  </si>
-  <si>
     <t>Starsand</t>
   </si>
   <si>
-    <t>Hành động Phiêu lưu Mô phỏng</t>
-  </si>
-  <si>
-    <t>Tunnel Vision Studio</t>
-  </si>
-  <si>
     <t>Internet Cafe Simulator 2</t>
   </si>
   <si>
-    <t>Chiến thuật Mô phỏng</t>
-  </si>
-  <si>
-    <t>Cheesecake Dev</t>
-  </si>
-  <si>
     <t>Pantropy</t>
   </si>
   <si>
-    <t>Brain Stone GmbH</t>
-  </si>
-  <si>
     <t>No Man's Sky</t>
   </si>
   <si>
-    <t>Hành động Phiêu lưu</t>
-  </si>
-  <si>
-    <t>Hello Games</t>
+    <t>Far Cry 6</t>
+  </si>
+  <si>
+    <t>The Sims 4: Deluxe Edition</t>
+  </si>
+  <si>
+    <t>My Time at Sandrock</t>
+  </si>
+  <si>
+    <t>The Iron Oath</t>
+  </si>
+  <si>
+    <t>Jurassic World Evolution 2</t>
+  </si>
+  <si>
+    <t>Bus Simulator 21</t>
+  </si>
+  <si>
+    <t>TOGETHER BnB</t>
+  </si>
+  <si>
+    <t>Alien Shooter 2 - New Era</t>
+  </si>
+  <si>
+    <t>Nigel's Journey : A Working Day</t>
+  </si>
+  <si>
+    <t>Lost Wing</t>
+  </si>
+  <si>
+    <t>dummy/game20.jpg</t>
   </si>
 </sst>
 </file>
@@ -417,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A2:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,26 +420,23 @@
     <col min="2" max="2" width="30.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="3.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -456,7 +444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -464,102 +452,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>